<commit_message>
Cleaned urls for better scraping results.
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -47,10 +47,10 @@
     </r>
   </si>
   <si>
-    <t>https://www.amazon.de/Apple-Smartwatch-Titangeh%C3%A4use-Fitnesstracker-Batterielaufzeit/dp/B0CHX1KZL9?th=1</t>
-  </si>
-  <si>
-    <t>https://www.ebay.de/itm/285702739821?_skw=apple+watch+ultra+2&amp;epid=5062783066&amp;itmmeta=01JGHQW2KHN4H7XPRJKST4VFA2&amp;hash=item428535d76d:g:D8kAAOSw1xpnB8LM&amp;itmprp=enc%3AAQAJAAAA0HoV3kP08IDx%2BKZ9MfhVJKnmrzhAbVJms7Lu7KYtDmaiqkFbxZ158mh%2Fro5uy9knrmFFn7F7CJnkbUPGGl6SzkN8G%2BtkvzQEcTGnETBt8rCwJu3xnL4BK9LcUcD34SowR8Z%2BE9ipBwS7FR2sFmsgoe8BKqTA3OSmlZjnGe7OHUk%2F6vyi6nORQXBozw3DAXPPed8%2FQjcA8c%2F5ANt0f1isQk0rYEVuc%2BWp%2B6sZLCogmQRa%2FtmvbhPqXaAPTKEKVvOP%2Fu3t7KhaKUCDQoAVYB%2BCgDk%3D%7Ctkp%3ABlBMUPSp8LeEZQ</t>
+    <t>https://www.amazon.de/Apple-Smartwatch-Titangeh%C3%A4use-Fitnesstracker-Batterielaufzeit/dp/B0CHX1KZL9</t>
+  </si>
+  <si>
+    <t>https://www.ebay.de/itm/285702739821</t>
   </si>
   <si>
     <t>Apple Watch Ultra</t>
@@ -70,7 +70,7 @@
     <t>https://www.amazon.de/Apple-Watch-Ultra-GPS-Cellular-49mm-Smartwatch/dp/B0BDJ3VKHD</t>
   </si>
   <si>
-    <t>https://www.ebay.de/itm/205170563909?_skw=apple+watch+ultra+medium&amp;epid=5056276766&amp;itmmeta=01JG45M91SGZPFED9RYHYQ9355&amp;hash=item2fc51e5b45:g:wcMAAOSwT-NnYeoa&amp;itmprp=enc%3AAQAJAAAA8HoV3kP08IDx%2BKZ9MfhVJKkK%2BaZpPoVOyATN743OVaM%2Bo9DHU3hatFLiN4OF1ZQdp6xVpGeTe24EyfsVsWLmxQlDgTY8jSlaID9c1zoaqPtJ2v055baBVBY%2FxlBsYRJW4glJ74WDK0sY%2Fgiu0hu5kyK9pI8TS2srwhG9sY13MV4YDZ%2BmRVlB3U%2FGeQl38zEaVo8lRS%2BoQNHZIIJO68Xx83njTWJcwcm2Bt5KS%2FVXNFQsBMrawsmuDiDdzmiC%2Bvt3HshXICH4lh8ANPbU3n0wtCNwSaFdHZmoT0UmVnPwda9bZEAMFB7TLgec5d9P2rPbOA%3D%3D%7Ctkp%3ABFBMhJHRhYFl</t>
+    <t>https://www.ebay.de/itm/205170563909</t>
   </si>
   <si>
     <t>Garmin Epix™ Pro Gen 2</t>
@@ -87,10 +87,10 @@
     </r>
   </si>
   <si>
-    <t>https://www.amazon.de/-/en/Sapphire-Performance-Technology-Flashlight-Whitestone-Titanium-Band/dp/B0BYFCRDT9/ref=sr_1_7?crid=33V50ZCHHMEJR&amp;dib=eyJ2IjoiMSJ9.9VUt4RUS9GeL46s_wKYD7NOzpk1RL7GFBTzGfl5hvNb5UoWM9_bE5cViLbexZ_sHgqOrFaHTiCiZsuzLi5NIWLQDYRG88SH38PCxmI3jB1h-eXipD291oPTkAzLEJpMBJ7DFiCoZ4p_ZMKrMW9wQLepydVU393cVaymP32CIMKPG09IL2sENb7b5fNgoLk7FyHeWLKRt78MUjNJEvYpMXQRVM0E8PcF2Wc4Rkfu3yeTCDBrdXBnMVutyGkvxi-UcIw_a7eefiIz31CnfT7-WQF8dVMkz0ikSd1TEL_ApHJIFTWIZPSjluqGTKaxfCnNn6MJuBUTXJt1xAm4LQSt1IZ0-8JvjloaoBb0GTx0_qqs.cPh5EYrAco41-y1UHmnWIn6XoGeErifdirnAFfzaUGI&amp;dib_tag=se&amp;keywords=Garmin%2Bepix%2BPro%2B(Gen%2B2)%2B47mm&amp;nsdOptOutParam=true&amp;qid=1735307304&amp;s=ce-de&amp;sprefix=garmin%2Bepix%2Bpro%2Bgen%2B2%2B47mm%2Celectronics%2C92&amp;sr=1-7&amp;th=1</t>
-  </si>
-  <si>
-    <t>https://www.ebay.de/itm/135341087540?_skw=garmin+epix+pro+gen+2+sapphire+47mm&amp;epid=4061457473&amp;itmmeta=01JG468WB7NAZNSCPJ2VG4HG4Y&amp;hash=item1f82f51b34:g:6PUAAOSwTTxnJ5zn&amp;itmprp=enc%3AAQAJAAABAHoV3kP08IDx%2BKZ9MfhVJKm6wo80sOBcVPZdRFmPojaFG8jk7e7WfcL5xDjd%2BI4BvdmUcFU3yHowcvnM5kROKOlHR4uWvIHbf%2BoasBuHUgGW50Pz%2BlQCk2s82%2FNfciwDVQ127P5Kh8hkKJ7c6MElWZnvfSSw4wPCUwIK6od2EZEMHs%2FLA12f1WpNmUgR2DnIOTTlYrgk5Vqap2qYRP8DOgDXCmaiJw9m1EScuak8N%2FRPsbEboKUKXVmeCidhiz6sekgsYokQKxagAwfguDvo3yrg1mBjlr5t3A5YGu1sKWk0deExyXxMrQisGGnYbk9u02j2ZP8VWvaJKTBAMjFGISg%3D%7Ctkp%3ABk9SR-TFo4aBZQ</t>
+    <t>https://www.amazon.de/Sapphire-Performance-Technology-Flashlight-Whitestone-Titanium-Band/dp/B0BYFCRDT9</t>
+  </si>
+  <si>
+    <t>https://www.ebay.de/itm/135341087540</t>
   </si>
   <si>
     <t>Garmin Venu 3S</t>
@@ -107,10 +107,10 @@
     </r>
   </si>
   <si>
-    <t>https://www.amazon.de/-/en/Bluetooth-Telephony-Assistance-Functions-Wheelchair/dp/B0CDC6Y617/ref=sr_1_1?crid=2Z49M7VGO2PHD&amp;dib=eyJ2IjoiMSJ9.zsozStpxjTb10_dqOgps1P7Ov9vHXMzLfv_2mBKuCgU5IvOJD8LIx_dc0D3Cn4-v25kyjQUwwwMJ9n4GQIrj6eOjdqxjXage6SKHeygkhTtDUuZNXTWpxvxOVa_LlYWJaeT9jlGCB1ja-JDbUPWGO0mLtUpdaQUKle0FoNur86RcthLO_P2Vqtxbhbzdo0XeaKp058QHfYPZ48Pf4v_CD1kRa6ogTZjEk6gBm6yYYcuDkn94yInRwn4wAuMs5j22M4mpNJopPrx-21k5r_Y4ntqKYFdPvtvAVT-DEc5vzkgKcfL8Ev6NgTemgB32TFWUOZ6QOKHNPRs8iFROr2jsttg5KXAeA7aCT7iDlbb7KGQ.fMhgWYRlmFGNv20An79v014xNx9NPU487reIA_M6QRA&amp;dib_tag=se&amp;keywords=garmin+venu+3s&amp;nsdOptOutParam=true&amp;qid=1735307840&amp;s=sports&amp;sprefix=garmin+venu+3s%2Csports%2C94&amp;sr=1-1</t>
-  </si>
-  <si>
-    <t>https://www.ebay.de/itm/396060223241?_skw=Garmin+Venu+3S&amp;itmmeta=01JG47VZ4PBGTGS1C1QN1Y9MQK&amp;hash=item5c37076709:g:nC8AAOSwrGRnbm8Y&amp;itmprp=enc%3AAQAJAAAA8HoV3kP08IDx%2BKZ9MfhVJKmfSWnxSsA2eW3Nn8S0JO75IwKFDMzGSpj8m260Z%2FkYx4r2kSu8dLBWy3fgw%2B4NUFLtVoANJP%2BAajSl4mUOglU2kWgAiJXHUxnDEUc%2Fvy97QpmCGGwVxcKT2vjOG89TG1KVe8nCrvHKeyRL37kp04%2BFffoLaaE4FCT16hmHYykYmu%2FptXmRC6geak38KSlV6biZPHxCd2Nn2ncQpusoZt3l%2BdeHa54W2AnvxVuuWnkep9HRHp6cbhnq1OGcQFefurbCKjB6%2BglU9U4vX0pFqv3oTLZiy3NSpvulR7D9kkjO5w%3D%3D%7Ctkp%3ABk9SR9Ty74eBZQ</t>
+    <t>https://www.amazon.de/Bluetooth-Telephony-Assistance-Functions-Wheelchair/dp/B0CDC6Y617</t>
+  </si>
+  <si>
+    <t>https://www.ebay.de/itm/396060223241</t>
   </si>
   <si>
     <t>Garmin Venu 3</t>
@@ -127,10 +127,10 @@
     </r>
   </si>
   <si>
-    <t>https://www.amazon.de/-/en/gp/product/B0CDC6H66Y/ref=ox_sc_act_title_1?smid=A3CNCH5ACJE9HG&amp;th=1</t>
-  </si>
-  <si>
-    <t>https://www.ebay.de/itm/356171896325?_trkparms=amclksrc%3DITM%26aid%3D1110018%26algo%3DHOMESPLICE.COMPLISTINGS%26ao%3D1%26asc%3D277989%2C278304%26meid%3D89a5d397238443e69199863d1ab32bec%26pid%3D101196%26rk%3D3%26rkt%3D12%26sd%3D405443443930%26itm%3D356171896325%26pmt%3D1%26noa%3D0%26pg%3D2332490%26algv%3DCompVIDesktopATF2V6%26brand%3DGarmin&amp;_trksid=p2332490.c101196.m2219&amp;itmprp=cksum%3A35617189632589a5d397238443e69199863d1ab32bec%7Cenc%3AAQAJAAABELx1mZQ2L9jLv%252BUPTFTna8XcGfl2wNJcn022gtZb5sDibGeq85%252BxT%252FnnZ4LZzMVPpz%252FR2qXUjr3O%252B3pMAPsNzfVJWiYukUUAvdpEVdACadQuf1wFYsnJrfKe1MeDqtz4%252FiL%252FIgY5rYPtzra4noaHfS7QHhsJqFo4rHOUlzeQTh8LqRrPC01gTr3DN7i0dR0HYU5mOO9ApSBdIwcj7K7gGLhg%252BnZHgHj3EFcSbp53bScx4YneA4QIqcYr0BvO7aABGeYDG4N5IOpz28fnOIrfeNC3fPMcxr17XUO9hZ2VPXttCcMWpCgcbZyI3HKX%252BpHoPCSqtHi9uM4SoM5m87kwdMx28zUArDidk6aE0UBuLEcl%7Campid%3APL_CLK%7Cclp%3A2332490&amp;epid=17034381920&amp;itmmeta=01JG46R6TNHRR4B1TJEKE0280G</t>
+    <t>https://www.amazon.de/gp/product/B0CDC6H66Y</t>
+  </si>
+  <si>
+    <t>https://www.ebay.de/itm/356171896325</t>
   </si>
   <si>
     <t>Garmin fēnix® 7X Pro</t>
@@ -147,10 +147,10 @@
     </r>
   </si>
   <si>
-    <t>https://www.amazon.de/-/en/Garmin-f%C4%93nix-Pro-Multisport-Pre-Installed/dp/B0C3WCGVQ3/ref=sr_1_1?dib=eyJ2IjoiMSJ9.XZnvKtjh-WYMF6p42K3ncSRJuZrO3LzNdMDjmBvKDQBgVMN81An27XXLncEL9beYgaeeEDgLR0Ir-zYvqmv6aeWUSZLk5_ix-x-9qaXweyTgQzJRxo861CXUxcmsXqPt2TQfJSpn0WklOpk1myLVoAN5-IhK4-N2AtGn62JHC0aY2hiQrEqe-KNo-XllW0uWaf5meZiyJuYEHekaz2Yzz7gcRFVMrC2uqN6jvyF_7Xg.nsu7O4Wo60Rt0WnamqLLZqZOVlTqTpRanYFXUbv_Xb4&amp;dib_tag=se&amp;keywords=Garmin%2Bf%C4%93nix%2B7X%2BPro&amp;m=A133RA3ZUAU4I7&amp;nsdOptOutParam=true&amp;qid=1735493741&amp;s=merchant-items&amp;sr=1-1&amp;th=1</t>
-  </si>
-  <si>
-    <t>https://www.ebay.de/itm/326337311619?var=0&amp;mkevt=1&amp;mkcid=1&amp;mkrid=707-53477-19255-0&amp;toolid=20006&amp;campid=5337770552&amp;customid=0Ly4lkxH8QqD4iAXbZTm6A</t>
+    <t>https://www.amazon.de/Garmin-f%C4%93nix-Pro-Multisport-Pre-Installed/dp/B0C3WCGVQ3</t>
+  </si>
+  <si>
+    <t>https://www.ebay.de/itm/326337311619</t>
   </si>
   <si>
     <t>Garmin fēnix® 7 Pro</t>
@@ -167,10 +167,10 @@
     </r>
   </si>
   <si>
-    <t>https://www.amazon.de/-/en/gp/product/B0C3WBJX4F/ref=ewc_pr_img_1?smid=A301WKE65PGVT5&amp;th=1</t>
-  </si>
-  <si>
-    <t>https://www.ebay.de/itm/186849889975?_skw=Garmin+f%C4%93nix+7+Pro&amp;itmmeta=01JG47476Y13YQJNE234VMTQN2&amp;hash=item2b811f0eb7:g:PKcAAOSwLwVnZBzt&amp;itmprp=enc%3AAQAJAAAA8HoV3kP08IDx%2BKZ9MfhVJKk6oMjbF9O1kJcsaRwAum0x%2FW1oUnCIWK2x4oCCjpgqGUmw6r540tVbcYf3jtohbn6p0kyuCTfu7yNTu3PT7C3m0yuCjEbzQKUzFobv1nFe2zbXCJ7bXnRvYyhpACIRuKTOcy0VqhoxOKxHTy42CtaEiVVtH%2BVE4AAdQ1eHuSl2BjHVg9mEX4ppghf06XhXWLb3hHfisNajPPw8GF9Bs7OFM%2Fe4uZl53ALSrV4n3p%2Bdgzy5Jf91q6KCIxJR%2BbP%2FWFUy%2Bg3da7teQP7LyMkC4ZMDxgUETRiCnwuo5gbxNecA5g%3D%3D%7Ctkp%3ABk9SR87zkIeBZQ</t>
+    <t>https://www.amazon.de/gp/product/B0C3WBJX4F</t>
+  </si>
+  <si>
+    <t>https://www.ebay.de/itm/186849889975</t>
   </si>
   <si>
     <t>Garmin Forerunner 965</t>
@@ -187,10 +187,10 @@
     </r>
   </si>
   <si>
-    <t>https://www.amazon.de/-/en/Forerunner%C2%AE-Colourful-Training-Recovery-010-02809-00-Black-powder-grey/dp/B0BS1TP8TJ?th=1</t>
-  </si>
-  <si>
-    <t>https://www.ebay.de/itm/387759330619?_skw=Garmin+Forerunner+965&amp;epid=18060107515&amp;itmmeta=01JG479K4S0TM0PXTBMDPNGZ5V&amp;hash=item5a4841d53b:g:ONcAAOSwQypnaoWE&amp;itmprp=enc%3AAQAJAAAA8HoV3kP08IDx%2BKZ9MfhVJKknTiv6roajmGUKtMKPpKj1wzEcuinae2egHVZqqFapdQyO2MFhhKNUty2qHBSwY9jLMwos1Acr8SEgyFwJ%2FBuhKBoEqWeRPfDkgtvBNVx8P%2Fn3HDI3QV1NHz%2B3Klbqizhy9aRRKIjrC7yPAUk2ksGpN%2B9jjl739tfn9gT6fgtvNwr%2F4PWufpt%2Fo3D7ivWVSqSto9XpOVFhMFnd1DMc%2BQJrJl0V5apsNkvBN03xhBOXTr30i0XyOEixehtiIFmZJ8cp4%2FJtohUyD4LLv3ClXxlUf7nMHZt5OlhQbXs0elrN0w%3D%3D%7Ctkp%3ABk9SR8aypoeBZQ</t>
+    <t>https://www.amazon.de/Forerunner%C2%AE-Colourful-Training-Recovery-010-02809-00-Black-powder-grey/dp/B0BS1TP8TJ</t>
+  </si>
+  <si>
+    <t>https://www.ebay.de/itm/387759330619</t>
   </si>
   <si>
     <t>Garmin Forerunner 255</t>
@@ -207,10 +207,10 @@
     </r>
   </si>
   <si>
-    <t>https://www.amazon.de/-/en/Garmin-Forerunner-Music-6817352319055-40181769666639-Black/dp/B0B2WY7TTH</t>
-  </si>
-  <si>
-    <t>https://www.ebay.de/itm/365283134351?_skw=Garmin+Forerunner+255&amp;itmmeta=01JG47FB9BBXV6GDBA7SZH1G7B&amp;hash=item550c924b8f:g:LV4AAOSwMCtnWswv&amp;itmprp=enc%3AAQAJAAAA8HoV3kP08IDx%2BKZ9MfhVJKlxbt6aSdqM9Ph50xMLcaGjRC60B%2BiAf4F1Xl1HPw3v%2Bs4Yo1ktZpArPz7bwYOPrMOww2ZkGy8pk4fbY%2FNCUGZOvhzO6hnOGHXWnQFJUVN4vx8qT2pSaVOgb0q5zE%2FqJuBsLKEs2DT3g6DZTm6UpF9Qk1hv5K8JF2pGGXwIveRTojZwQr8zqSa4gdKXajWfBFEvB%2BE9Qarv4Z07JtqFaZ%2FAP8tOXFq1rW7n5q1Esp7mcAQ9g1ZDS5itP5SvfuwKgjvuxt1E8uUgsIMg3CycGEaOFKdQ5sIQLvCVEwg2P3Mrsw%3D%3D%7Ctkp%3ABk9SR-i0vYeBZQ</t>
+    <t>https://www.amazon.de/Garmin-Forerunner-Music-6817352319055-40181769666639-Black/dp/B0B2WY7TTH</t>
+  </si>
+  <si>
+    <t>https://www.ebay.de/itm/365283134351</t>
   </si>
   <si>
     <t>Withings ScanWatch 2</t>
@@ -227,17 +227,17 @@
     </r>
   </si>
   <si>
-    <t>https://www.amazon.de/-/en/ScanWatch-Cardiovascular-Monitoring-Temperature-Variations/dp/B0CG9P8YFW?th=1</t>
-  </si>
-  <si>
-    <t>https://www.ebay.de/itm/267104675871?_skw=Withings+ScanWatch+2+38mm&amp;itmmeta=01JG47QMB4ZEYZB7SVTDPWPZGW&amp;hash=item3e30ade81f:g:vgwAAOSwV71naYdh&amp;itmprp=enc%3AAQAJAAAA4HoV3kP08IDx%2BKZ9MfhVJKnTmnD%2F1jnZw%2B9lys1EvN9MEQ5Yutjrf1cs3az4n%2BMx--X5JzaDu5Pssobu2FAf4n1Qv6tfO2HraidGHaZIxlT%2BZv5SbG7EX%2FPJ3ZulIrrQh9ShsGwuV0kp0WJAdeUDxnQ5IcEUe2vLnLdBJPVKoqGs0wDirRhdGTcg5oDRAXYKootIqJrtYSFmylo01JBTn8XLacvPSU9r9l7uobnA9en%2FXATeaWl7TDIvDIzCq5CRYCkHlJAOr0HuT1TDWdCKsTLTIhJTOkumQfLcqm73j3f%2F%7Ctkp%3ABk9SR9zF3oeBZQ</t>
+    <t>https://www.amazon.de/ScanWatch-Cardiovascular-Monitoring-Temperature-Variations/dp/B0CG9P8YFW</t>
+  </si>
+  <si>
+    <t>https://www.ebay.de/itm/267104675871</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -259,6 +259,12 @@
       <u/>
       <sz val="11.0"/>
       <color rgb="FF1155CC"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -296,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -308,6 +314,9 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -527,9 +536,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="26.0"/>
-    <col customWidth="1" min="2" max="2" width="26.14"/>
-    <col customWidth="1" min="3" max="3" width="32.86"/>
-    <col customWidth="1" min="4" max="4" width="20.29"/>
+    <col customWidth="1" min="2" max="2" width="43.14"/>
+    <col customWidth="1" min="3" max="3" width="55.14"/>
+    <col customWidth="1" min="4" max="4" width="39.14"/>
     <col customWidth="1" min="5" max="5" width="12.71"/>
     <col customWidth="1" min="6" max="26" width="8.71"/>
   </cols>
@@ -578,7 +587,7 @@
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="2">
@@ -592,10 +601,10 @@
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="2">
@@ -609,10 +618,10 @@
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="2">
@@ -626,10 +635,10 @@
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="2">
@@ -643,10 +652,10 @@
       <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E7" s="2">
@@ -660,10 +669,10 @@
       <c r="B8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="2">
@@ -677,10 +686,10 @@
       <c r="B9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E9" s="2">
@@ -694,10 +703,10 @@
       <c r="B10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="2">
@@ -711,10 +720,10 @@
       <c r="B11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>44</v>
       </c>
       <c r="E11" s="2">

</xml_diff>

<commit_message>
code updated all files
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\udwal\price-collection\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FDA9B9-B7E9-403E-9920-5169A454A245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1480" yWindow="1480" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="BHRifNxkSEpD85NEqoPD34vyoMGo4w+pCBajzLrngNA="/>
@@ -30,18 +39,15 @@
     <t>Ebay URL</t>
   </si>
   <si>
-    <t>G7 Price</t>
-  </si>
-  <si>
     <t>Apple Watch Ultra 2</t>
   </si>
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>https://www.idealo.de/preisvergleich/OffersOfProduct/203244685_-watch-ultra-2-apple.html</t>
     </r>
@@ -58,10 +64,10 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>https://www.idealo.de/preisvergleich/OffersOfProduct/202094481_-watch-ultra-apple.html</t>
     </r>
@@ -78,10 +84,10 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>https://www.idealo.de/preisvergleich/OffersOfProduct/202836311_-epix-pro-gen-2-garmin.html</t>
     </r>
@@ -98,10 +104,10 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>https://www.idealo.de/preisvergleich/OffersOfProduct/203216729_-venu-3s-garmin.html</t>
     </r>
@@ -118,10 +124,10 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>https://www.idealo.de/preisvergleich/OffersOfProduct/203216760_-venu-3-garmin.html</t>
     </r>
@@ -138,10 +144,10 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>https://www.idealo.de/preisvergleich/OffersOfProduct/202837116_-fnix-7x-pro-garmin.html</t>
     </r>
@@ -158,10 +164,10 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>https://www.idealo.de/preisvergleich/OffersOfProduct/202837359_-fnix-7-pro-garmin.html</t>
     </r>
@@ -178,10 +184,10 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>https://www.idealo.de/preisvergleich/OffersOfProduct/202365010_-forerunner-965-garmin.html</t>
     </r>
@@ -198,10 +204,10 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>https://www.idealo.de/preisvergleich/OffersOfProduct/201979106_-forerunner-255-garmin.html</t>
     </r>
@@ -218,10 +224,10 @@
   <si>
     <r>
       <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
         <rFont val="Calibri, sans-serif"/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
       </rPr>
       <t>https://www.idealo.de/preisvergleich/OffersOfProduct/203380026_-scanwatch-2-withings.html</t>
     </r>
@@ -231,47 +237,57 @@
   </si>
   <si>
     <t>https://www.ebay.de/itm/267104675871</t>
+  </si>
+  <si>
+    <t>G7 Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF1155CC"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF1155CC"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF1155CC"/>
+      <name val="Calibri, sans-serif"/>
     </font>
   </fonts>
   <fills count="2">
@@ -279,11 +295,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -297,42 +319,40 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -522,28 +542,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.0"/>
-    <col customWidth="1" min="2" max="2" width="43.14"/>
-    <col customWidth="1" min="3" max="3" width="68.71"/>
-    <col customWidth="1" min="4" max="4" width="39.14"/>
-    <col customWidth="1" min="5" max="5" width="12.71"/>
-    <col customWidth="1" min="6" max="26" width="8.71"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="43.08984375" customWidth="1"/>
+    <col min="3" max="3" width="68.7265625" customWidth="1"/>
+    <col min="4" max="4" width="39.08984375" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" customWidth="1"/>
+    <col min="6" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="14.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,174 +579,174 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.5">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="E2" s="2">
         <v>839.99</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="14.5">
       <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="E3" s="2">
         <v>689.99</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" ht="14.5">
       <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="E4" s="2">
         <v>699.99</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" ht="14.5">
       <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="E5" s="2">
         <v>389.99</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" ht="14.5">
       <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="E6" s="2">
         <v>409.99</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" ht="14.5">
       <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="E7" s="2">
         <v>699.99</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" ht="14.5">
       <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="E8" s="2">
         <v>619.99</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" ht="14.5">
       <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="E9" s="2">
         <v>559.99</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" ht="14.5">
       <c r="A10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="E10" s="2">
         <v>239.99</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" ht="14.5">
       <c r="A11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="E11" s="2">
         <v>129.99</v>
@@ -1712,40 +1734,38 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="C2"/>
-    <hyperlink r:id="rId3" ref="D2"/>
-    <hyperlink r:id="rId4" ref="B3"/>
-    <hyperlink r:id="rId5" ref="C3"/>
-    <hyperlink r:id="rId6" ref="D3"/>
-    <hyperlink r:id="rId7" ref="B4"/>
-    <hyperlink r:id="rId8" ref="C4"/>
-    <hyperlink r:id="rId9" ref="D4"/>
-    <hyperlink r:id="rId10" ref="B5"/>
-    <hyperlink r:id="rId11" ref="C5"/>
-    <hyperlink r:id="rId12" ref="D5"/>
-    <hyperlink r:id="rId13" ref="B6"/>
-    <hyperlink r:id="rId14" ref="C6"/>
-    <hyperlink r:id="rId15" ref="D6"/>
-    <hyperlink r:id="rId16" ref="B7"/>
-    <hyperlink r:id="rId17" ref="C7"/>
-    <hyperlink r:id="rId18" ref="D7"/>
-    <hyperlink r:id="rId19" ref="B8"/>
-    <hyperlink r:id="rId20" ref="C8"/>
-    <hyperlink r:id="rId21" ref="D8"/>
-    <hyperlink r:id="rId22" ref="B9"/>
-    <hyperlink r:id="rId23" ref="C9"/>
-    <hyperlink r:id="rId24" ref="D9"/>
-    <hyperlink r:id="rId25" ref="B10"/>
-    <hyperlink r:id="rId26" ref="C10"/>
-    <hyperlink r:id="rId27" ref="D10"/>
-    <hyperlink r:id="rId28" ref="B11"/>
-    <hyperlink r:id="rId29" ref="C11"/>
-    <hyperlink r:id="rId30" ref="D11"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B4" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C4" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D4" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B5" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C5" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D5" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B6" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C6" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D6" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B7" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C7" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D7" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B8" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C8" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D8" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B9" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C9" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D9" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B10" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C10" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="D10" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B11" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C11" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="D11" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
   </hyperlinks>
-  <printOptions/>
-  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>